<commit_message>
fix api import point list
</commit_message>
<xml_diff>
--- a/error-import-demo-point-list.xlsx
+++ b/error-import-demo-point-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Boku no\InternshipProject\student-fita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC91D780-387C-4BCC-BEDA-0DC29248F97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF655BE2-E536-4C92-A30B-826862CDED5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0A5968B0-B636-4779-A398-BA415D297B06}"/>
   </bookViews>
@@ -107,8 +107,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>20242</v>
+        <v>20222</v>
       </c>
       <c r="C2" s="3">
         <v>8.91</v>
@@ -486,11 +486,11 @@
       </c>
       <c r="E2" s="3">
         <f t="shared" ref="E2:E7" ca="1" si="0">RANDBETWEEN(25,130)</f>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" ref="F2:F7" ca="1" si="1">RANDBETWEEN(50,100)</f>
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G2" s="3">
         <v>8.9600000000000009</v>
@@ -514,11 +514,11 @@
       </c>
       <c r="E3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="G3" s="3">
         <v>7.18</v>
@@ -532,7 +532,7 @@
         <v>6652385</v>
       </c>
       <c r="B4" s="3">
-        <v>20242</v>
+        <v>20222</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -542,11 +542,11 @@
       </c>
       <c r="E4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G4" s="3">
         <v>6.07</v>
@@ -560,7 +560,7 @@
         <v>6655419</v>
       </c>
       <c r="B5" s="3">
-        <v>20242</v>
+        <v>20222</v>
       </c>
       <c r="C5" s="3">
         <v>1.95</v>
@@ -570,11 +570,11 @@
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G5" s="3">
         <v>1.96</v>
@@ -588,7 +588,7 @@
         <v>6667532</v>
       </c>
       <c r="B6" s="3">
-        <v>20211</v>
+        <v>20222</v>
       </c>
       <c r="C6" s="3">
         <v>9.19</v>
@@ -598,11 +598,11 @@
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G6" s="3">
         <v>9.24</v>
@@ -616,7 +616,7 @@
         <v>6666130</v>
       </c>
       <c r="B7" s="3">
-        <v>20242</v>
+        <v>20222</v>
       </c>
       <c r="C7" s="3">
         <v>0.6</v>
@@ -626,11 +626,11 @@
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="G7" s="3">
         <v>0.61</v>

</xml_diff>